<commit_message>
New template and clean questions
</commit_message>
<xml_diff>
--- a/templates/questions.xlsx
+++ b/templates/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b235f5438060bce/Documentos/Development/500Historias/trivia/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b235f5438060bce/Documentos/Development/500Historias/trivia2/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{273BC620-7E6C-416A-A137-4E1D81F35F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{380490D4-2A94-420E-A865-4ECA286600FD}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{273BC620-7E6C-416A-A137-4E1D81F35F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D754E7-9504-4BE1-9865-CA6CCDD6FC19}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{9721EB32-687B-4607-9B19-EB20297D65DC}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="517">
   <si>
     <t>Correcta</t>
   </si>
@@ -1542,6 +1542,144 @@
   </si>
   <si>
     <t>Pedro</t>
+  </si>
+  <si>
+    <t>¿Quién fue el héroe que mató a la Hidra en la mitología griega?</t>
+  </si>
+  <si>
+    <t>¿Como se llama el reino del dios de los muertos en la mitologia griega?</t>
+  </si>
+  <si>
+    <t>¿Quién fue el hombre que se enamoró de su propia imagen en la mitología griega?</t>
+  </si>
+  <si>
+    <t>¿Qué autor escribió "El Aleph"?</t>
+  </si>
+  <si>
+    <t>¿Qué autor escribió "El llano en llamas"?</t>
+  </si>
+  <si>
+    <t>¿De qué país es originario el personaje de "El Silbón"?</t>
+  </si>
+  <si>
+    <t>¿Qué libro de Mario Vargas Llosa fue adaptado al cine?</t>
+  </si>
+  <si>
+    <t>¿Quién escribió "El amor en los tiempos del cólera"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de "La Continuidad de los Parques"?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de García Márquez que cuenta la historia de la familia Buendía?</t>
+  </si>
+  <si>
+    <t>¿Quién escribió el libro "Rayuela"?</t>
+  </si>
+  <si>
+    <t>¿De qué libro de García Márquez es famoso el personaje de Remedios La Bella?</t>
+  </si>
+  <si>
+    <t>¿Cuál novela de Julio Cortázar narra la historia de Horacio Oliveira?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de J. L. Borges cuenta la historia de una biblioteca infinita?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de la trilogía "El señor de los anillos"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el personaje principal en "Los juegos del hambre"?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el título del primer libro de la saga "Canción de hielo y fuego"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de la saga de libros "Canción de hielo y fuego"?</t>
+  </si>
+  <si>
+    <t>El pueblo de Israel</t>
+  </si>
+  <si>
+    <t>El cuy</t>
+  </si>
+  <si>
+    <t>El camello</t>
+  </si>
+  <si>
+    <t>La alpaca</t>
+  </si>
+  <si>
+    <t>La llama</t>
+  </si>
+  <si>
+    <t>La pata del diablo</t>
+  </si>
+  <si>
+    <t>Chichen Itzá</t>
+  </si>
+  <si>
+    <t>La familia y el pecado</t>
+  </si>
+  <si>
+    <t>¿Quién mató a Palomino Molero?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Vargas Llosa comienza con el descubrimiento del cuerpo de un joven aviador?</t>
+  </si>
+  <si>
+    <t>El Aleph</t>
+  </si>
+  <si>
+    <t>la noche boca arriba</t>
+  </si>
+  <si>
+    <t>El prisionero de Askaban</t>
+  </si>
+  <si>
+    <t>H.P. y el cáliz de fuego</t>
+  </si>
+  <si>
+    <t>Harry Potter y la camara secreta</t>
+  </si>
+  <si>
+    <t>El Gran Lebowski</t>
+  </si>
+  <si>
+    <t>Catnip Evergreen</t>
+  </si>
+  <si>
+    <t>Buzz Lightyear</t>
+  </si>
+  <si>
+    <t>City of bones</t>
+  </si>
+  <si>
+    <t>El Mago de Oz</t>
+  </si>
+  <si>
+    <t>La biblioteca de Morel</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Rosa María Britton habla de una mujer que vive en la selva panameña?</t>
+  </si>
+  <si>
+    <t>¿Qué leyenda latinoamericana cuenta la historia de un hombre que vende su alma al diablo?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Stephen King sigue a un grupo de niños enfrentando a un payaso?</t>
+  </si>
+  <si>
+    <t>¿Novela de Rose Marie Tapia que narra el impacto de la crisis económica y social en una familia común?</t>
+  </si>
+  <si>
+    <t>¿Qué libro de Paulo Coelho cuenta la historia de un joven y su viaje espiritual?</t>
+  </si>
+  <si>
+    <t>¿Qué leyenda latinoamericana cuenta la historia de una mujer que llora por sus hijos?</t>
+  </si>
+  <si>
+    <t>¿Cuál novela de Isabel Allende cuenta la historia de una familia durante la dictadura de Pinochet?</t>
   </si>
 </sst>
 </file>
@@ -1573,12 +1711,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1593,13 +1737,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,12 +2063,12 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="129.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.23046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.07421875" bestFit="1" customWidth="1"/>
@@ -1948,7 +2094,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>471</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2050,7 +2196,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>472</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -2067,7 +2213,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>473</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -2093,7 +2239,7 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>489</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -2223,16 +2369,16 @@
         <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>493</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>492</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>491</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -2270,11 +2416,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>91</v>
+      <c r="A21" s="5" t="s">
+        <v>511</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>494</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -2287,8 +2433,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>96</v>
+      <c r="A22" s="5" t="s">
+        <v>515</v>
       </c>
       <c r="B22" t="s">
         <v>97</v>
@@ -2297,7 +2443,7 @@
         <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>495</v>
       </c>
       <c r="E22" t="s">
         <v>100</v>
@@ -2305,7 +2451,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>474</v>
       </c>
       <c r="B23" t="s">
         <v>102</v>
@@ -2322,7 +2468,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>475</v>
       </c>
       <c r="B24" t="s">
         <v>106</v>
@@ -2339,7 +2485,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>476</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -2373,7 +2519,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>477</v>
       </c>
       <c r="B27" t="s">
         <v>119</v>
@@ -2390,7 +2536,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>478</v>
       </c>
       <c r="B28" t="s">
         <v>116</v>
@@ -2407,7 +2553,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>479</v>
       </c>
       <c r="B29" t="s">
         <v>125</v>
@@ -2424,7 +2570,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>514</v>
       </c>
       <c r="B30" t="s">
         <v>127</v>
@@ -2441,13 +2587,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>480</v>
       </c>
       <c r="B31" t="s">
         <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>496</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -2458,7 +2604,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>481</v>
       </c>
       <c r="B32" t="s">
         <v>125</v>
@@ -2475,10 +2621,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>498</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>497</v>
       </c>
       <c r="C33" t="s">
         <v>122</v>
@@ -2492,13 +2638,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>482</v>
       </c>
       <c r="B34" t="s">
         <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>133</v>
+        <v>499</v>
       </c>
       <c r="D34" t="s">
         <v>142</v>
@@ -2526,7 +2672,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>516</v>
       </c>
       <c r="B36" t="s">
         <v>147</v>
@@ -2538,18 +2684,18 @@
         <v>149</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>483</v>
       </c>
       <c r="B37" t="s">
         <v>152</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>500</v>
       </c>
       <c r="D37" t="s">
         <v>154</v>
@@ -2577,13 +2723,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>484</v>
       </c>
       <c r="B39" t="s">
         <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>509</v>
       </c>
       <c r="D39" t="s">
         <v>161</v>
@@ -2594,7 +2740,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>510</v>
       </c>
       <c r="B40" t="s">
         <v>164</v>
@@ -2644,8 +2790,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>176</v>
+      <c r="A43" s="4" t="s">
+        <v>513</v>
       </c>
       <c r="B43" t="s">
         <v>177</v>
@@ -2685,18 +2831,18 @@
         <v>186</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
+        <v>501</v>
       </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>502</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>503</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>485</v>
       </c>
       <c r="B46" t="s">
         <v>190</v>
@@ -2716,7 +2862,7 @@
         <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>457</v>
       </c>
       <c r="C47" t="s">
         <v>196</v>
@@ -2730,7 +2876,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>487</v>
       </c>
       <c r="B48" t="s">
         <v>200</v>
@@ -2747,19 +2893,19 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>486</v>
       </c>
       <c r="B49" t="s">
         <v>205</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>505</v>
       </c>
       <c r="D49" t="s">
-        <v>207</v>
+        <v>504</v>
       </c>
       <c r="E49" t="s">
-        <v>208</v>
+        <v>506</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
@@ -2767,13 +2913,13 @@
         <v>209</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>507</v>
       </c>
       <c r="C50" t="s">
         <v>211</v>
       </c>
       <c r="D50" t="s">
-        <v>212</v>
+        <v>508</v>
       </c>
       <c r="E50" t="s">
         <v>213</v>
@@ -2781,7 +2927,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>488</v>
       </c>
       <c r="B51" t="s">
         <v>193</v>
@@ -2865,8 +3011,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>236</v>
+      <c r="A56" s="5" t="s">
+        <v>512</v>
       </c>
       <c r="B56" t="s">
         <v>237</v>

</xml_diff>

<commit_message>
New templates and questions
</commit_message>
<xml_diff>
--- a/templates/questions.xlsx
+++ b/templates/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b235f5438060bce/Documentos/Development/500Historias/trivia/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b235f5438060bce/Documentos/Development/500Historias/trivia2/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{273BC620-7E6C-416A-A137-4E1D81F35F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{380490D4-2A94-420E-A865-4ECA286600FD}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{273BC620-7E6C-416A-A137-4E1D81F35F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D754E7-9504-4BE1-9865-CA6CCDD6FC19}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{9721EB32-687B-4607-9B19-EB20297D65DC}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="517">
   <si>
     <t>Correcta</t>
   </si>
@@ -1542,6 +1542,144 @@
   </si>
   <si>
     <t>Pedro</t>
+  </si>
+  <si>
+    <t>¿Quién fue el héroe que mató a la Hidra en la mitología griega?</t>
+  </si>
+  <si>
+    <t>¿Como se llama el reino del dios de los muertos en la mitologia griega?</t>
+  </si>
+  <si>
+    <t>¿Quién fue el hombre que se enamoró de su propia imagen en la mitología griega?</t>
+  </si>
+  <si>
+    <t>¿Qué autor escribió "El Aleph"?</t>
+  </si>
+  <si>
+    <t>¿Qué autor escribió "El llano en llamas"?</t>
+  </si>
+  <si>
+    <t>¿De qué país es originario el personaje de "El Silbón"?</t>
+  </si>
+  <si>
+    <t>¿Qué libro de Mario Vargas Llosa fue adaptado al cine?</t>
+  </si>
+  <si>
+    <t>¿Quién escribió "El amor en los tiempos del cólera"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de "La Continuidad de los Parques"?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de García Márquez que cuenta la historia de la familia Buendía?</t>
+  </si>
+  <si>
+    <t>¿Quién escribió el libro "Rayuela"?</t>
+  </si>
+  <si>
+    <t>¿De qué libro de García Márquez es famoso el personaje de Remedios La Bella?</t>
+  </si>
+  <si>
+    <t>¿Cuál novela de Julio Cortázar narra la historia de Horacio Oliveira?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de J. L. Borges cuenta la historia de una biblioteca infinita?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de la trilogía "El señor de los anillos"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el personaje principal en "Los juegos del hambre"?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el título del primer libro de la saga "Canción de hielo y fuego"?</t>
+  </si>
+  <si>
+    <t>¿Quién es el autor de la saga de libros "Canción de hielo y fuego"?</t>
+  </si>
+  <si>
+    <t>El pueblo de Israel</t>
+  </si>
+  <si>
+    <t>El cuy</t>
+  </si>
+  <si>
+    <t>El camello</t>
+  </si>
+  <si>
+    <t>La alpaca</t>
+  </si>
+  <si>
+    <t>La llama</t>
+  </si>
+  <si>
+    <t>La pata del diablo</t>
+  </si>
+  <si>
+    <t>Chichen Itzá</t>
+  </si>
+  <si>
+    <t>La familia y el pecado</t>
+  </si>
+  <si>
+    <t>¿Quién mató a Palomino Molero?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Vargas Llosa comienza con el descubrimiento del cuerpo de un joven aviador?</t>
+  </si>
+  <si>
+    <t>El Aleph</t>
+  </si>
+  <si>
+    <t>la noche boca arriba</t>
+  </si>
+  <si>
+    <t>El prisionero de Askaban</t>
+  </si>
+  <si>
+    <t>H.P. y el cáliz de fuego</t>
+  </si>
+  <si>
+    <t>Harry Potter y la camara secreta</t>
+  </si>
+  <si>
+    <t>El Gran Lebowski</t>
+  </si>
+  <si>
+    <t>Catnip Evergreen</t>
+  </si>
+  <si>
+    <t>Buzz Lightyear</t>
+  </si>
+  <si>
+    <t>City of bones</t>
+  </si>
+  <si>
+    <t>El Mago de Oz</t>
+  </si>
+  <si>
+    <t>La biblioteca de Morel</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Rosa María Britton habla de una mujer que vive en la selva panameña?</t>
+  </si>
+  <si>
+    <t>¿Qué leyenda latinoamericana cuenta la historia de un hombre que vende su alma al diablo?</t>
+  </si>
+  <si>
+    <t>¿Qué novela de Stephen King sigue a un grupo de niños enfrentando a un payaso?</t>
+  </si>
+  <si>
+    <t>¿Novela de Rose Marie Tapia que narra el impacto de la crisis económica y social en una familia común?</t>
+  </si>
+  <si>
+    <t>¿Qué libro de Paulo Coelho cuenta la historia de un joven y su viaje espiritual?</t>
+  </si>
+  <si>
+    <t>¿Qué leyenda latinoamericana cuenta la historia de una mujer que llora por sus hijos?</t>
+  </si>
+  <si>
+    <t>¿Cuál novela de Isabel Allende cuenta la historia de una familia durante la dictadura de Pinochet?</t>
   </si>
 </sst>
 </file>
@@ -1573,12 +1711,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1593,13 +1737,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,12 +2063,12 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="129.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.23046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.07421875" bestFit="1" customWidth="1"/>
@@ -1948,7 +2094,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>471</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2050,7 +2196,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>472</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -2067,7 +2213,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>473</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -2093,7 +2239,7 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>489</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -2223,16 +2369,16 @@
         <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>493</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>492</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>491</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -2270,11 +2416,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>91</v>
+      <c r="A21" s="5" t="s">
+        <v>511</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>494</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -2287,8 +2433,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>96</v>
+      <c r="A22" s="5" t="s">
+        <v>515</v>
       </c>
       <c r="B22" t="s">
         <v>97</v>
@@ -2297,7 +2443,7 @@
         <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>495</v>
       </c>
       <c r="E22" t="s">
         <v>100</v>
@@ -2305,7 +2451,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>474</v>
       </c>
       <c r="B23" t="s">
         <v>102</v>
@@ -2322,7 +2468,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>475</v>
       </c>
       <c r="B24" t="s">
         <v>106</v>
@@ -2339,7 +2485,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>476</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -2373,7 +2519,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>477</v>
       </c>
       <c r="B27" t="s">
         <v>119</v>
@@ -2390,7 +2536,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>478</v>
       </c>
       <c r="B28" t="s">
         <v>116</v>
@@ -2407,7 +2553,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>479</v>
       </c>
       <c r="B29" t="s">
         <v>125</v>
@@ -2424,7 +2570,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>514</v>
       </c>
       <c r="B30" t="s">
         <v>127</v>
@@ -2441,13 +2587,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>480</v>
       </c>
       <c r="B31" t="s">
         <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>496</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -2458,7 +2604,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>481</v>
       </c>
       <c r="B32" t="s">
         <v>125</v>
@@ -2475,10 +2621,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>498</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>497</v>
       </c>
       <c r="C33" t="s">
         <v>122</v>
@@ -2492,13 +2638,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>482</v>
       </c>
       <c r="B34" t="s">
         <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>133</v>
+        <v>499</v>
       </c>
       <c r="D34" t="s">
         <v>142</v>
@@ -2526,7 +2672,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>516</v>
       </c>
       <c r="B36" t="s">
         <v>147</v>
@@ -2538,18 +2684,18 @@
         <v>149</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>483</v>
       </c>
       <c r="B37" t="s">
         <v>152</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>500</v>
       </c>
       <c r="D37" t="s">
         <v>154</v>
@@ -2577,13 +2723,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>484</v>
       </c>
       <c r="B39" t="s">
         <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>509</v>
       </c>
       <c r="D39" t="s">
         <v>161</v>
@@ -2594,7 +2740,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>510</v>
       </c>
       <c r="B40" t="s">
         <v>164</v>
@@ -2644,8 +2790,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>176</v>
+      <c r="A43" s="4" t="s">
+        <v>513</v>
       </c>
       <c r="B43" t="s">
         <v>177</v>
@@ -2685,18 +2831,18 @@
         <v>186</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
+        <v>501</v>
       </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>502</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>503</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>485</v>
       </c>
       <c r="B46" t="s">
         <v>190</v>
@@ -2716,7 +2862,7 @@
         <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>457</v>
       </c>
       <c r="C47" t="s">
         <v>196</v>
@@ -2730,7 +2876,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>487</v>
       </c>
       <c r="B48" t="s">
         <v>200</v>
@@ -2747,19 +2893,19 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>486</v>
       </c>
       <c r="B49" t="s">
         <v>205</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>505</v>
       </c>
       <c r="D49" t="s">
-        <v>207</v>
+        <v>504</v>
       </c>
       <c r="E49" t="s">
-        <v>208</v>
+        <v>506</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
@@ -2767,13 +2913,13 @@
         <v>209</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>507</v>
       </c>
       <c r="C50" t="s">
         <v>211</v>
       </c>
       <c r="D50" t="s">
-        <v>212</v>
+        <v>508</v>
       </c>
       <c r="E50" t="s">
         <v>213</v>
@@ -2781,7 +2927,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>488</v>
       </c>
       <c r="B51" t="s">
         <v>193</v>
@@ -2865,8 +3011,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>236</v>
+      <c r="A56" s="5" t="s">
+        <v>512</v>
       </c>
       <c r="B56" t="s">
         <v>237</v>

</xml_diff>